<commit_message>
adding useless feature for removing later
</commit_message>
<xml_diff>
--- a/data/features.xlsx
+++ b/data/features.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="560" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="550" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="All" sheetId="1" r:id="rId1"/>
+    <sheet name="Useless" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
   <si>
     <t>HT_DCPERIOD</t>
   </si>
@@ -260,6 +260,90 @@
   </si>
   <si>
     <t>CDLXSIDEGAP3METHODS</t>
+  </si>
+  <si>
+    <t>[('2h_CDLMATHOLD', 0.0), ('2h_CDLDOJI', 0.0), ('2h_CDLLADDERBOTTOM', 0.0), ('2h_CDLDRAGONFLYDOJI', 0.0), ('2h_CDLGRAVESTONEDOJI', 0.0), ('2h_CDLTAKURI', 0.0), ('2h_CDLENGULFING', 0.0), ('2h_CDLKICKING', 0.0), ('2h_CDLKICKINGBYLENGTH', 0.0), ('2h_HT_SINE', 0.0), ('2h_HT_TRENDMODE', 0.0), ('2h_CDL3OUTSIDE', 0.0), ('2h_CDLDARKCLOUDCOVER', 0.0), ('2h_DX', 0.0), ('2h_CDLMORNINGSTAR', 0.0), ('2h_CDLINNECK', 0.0), ('2h_CDLCOUNTERATTACK', 0.0), ('2h_CDL3STARSINSOUTH', 0.0), ('2h_CDLEVENINGDOJISTAR', 0.0), ('2h_CDLUPSIDEGAP2CROWS', 0.0), ('2h_CDLHARAMI', 0.0), ('2h_CDLABANDONEDBABY', 0.0), ('12h_RSI', 0.0), ('12h_CDLHIKKAKE', 0.0), ('12h_CDLMATHOLD', 0.0), ('12h_CDLBREAKAWAY', 0.0), ('12h_CDLDOJI', 0.0), ('12h_TRIX', 0.0), ('12h_CDLLADDERBOTTOM', 0.0), ('12h_CDLRISEFALL3METHODS', 0.0), ('12h_CDLHANGINGMAN', 0.0), ('12h_AROONOSC', 0.0), ('12h_MFI', 0.0), ('12h_CDLCONCEALBABYSWALL', 0.0), ('12h_CDLHAMMER', 0.0), ('12h_CDLLONGLINE', 0.0), ('12h_CDLLONGLEGGEDDOJI', 0.0), ('12h_CDL3LINESTRIKE', 0.0), ('12h_CDLSTALLEDPATTERN', 0.0), ('12h_CDLSHORTLINE', 0.0), ('12h_HT_DCPHASE', 0.0), ('12h_CDL3BLACKCROWS', 0.0), ('12h_CDLKICKING', 0.0), ('12h_CDLKICKINGBYLENGTH', 0.0), ('12h_HT_TRENDMODE', 0.0), ('12h_CDLIDENTICAL3CROWS', 0.0), ('12h_CDLDARKCLOUDCOVER', 0.0), ('12h_ADX', 0.0), ('12h_DX', 0.0), ('12h_CDLINNECK', 0.0), ('12h_CDLONNECK', 0.0), ('12h_CDLBELTHOLD', 0.0), ('12h_CDLCOUNTERATTACK', 0.0), ('12h_CDL3STARSINSOUTH', 0.0), ('12h_CDLUPSIDEGAP2CROWS', 0.0), ('12h_CDLTHRUSTING', 0.0), ('12h_CDLABANDONEDBABY', 0.0), ('12h_CDLHIGHWAVE', 0.0), ('12h_CDLSTICKSANDWICH', 0.0), ('12h_CDLSEPARATINGLINES', 0.003756276823238492), ('12h_HT_SINE', 0.009257156593133383), ('2h_CDLGAPSIDESIDEWHITE', -0.01386584544438379), ('2h_CDLSTICKSANDWICH', -0.01531186564737108), ('2h_CDLINVERTEDHAMMER', -0.030558377360614054), ('12h_CDLDOJISTAR', 0.033914071521249554), ('12h_STOCHF', 0.03519306895909331), ('12h_CDL3INSIDE', 0.03853514170349506), ('2h_CDLHIKKAKE', 0.04590047865208033), ('12h_CDLXSIDEGAP3METHODS', 0.05064224529817387), ('12h_CDLMARUBOZU', 0.055460647430801126), ('12h_CDLSPINNINGTOP', -0.06041224990932476), ('2h_CDLRICKSHAWMAN', -0.06076636116761273), ('2h_CDLSPINNINGTOP', -0.06787611729649656), ('12h_STOCHRSI', -0.07045724225824293), ('2h_CDLSHORTLINE', -0.07404094923707907), ('12h_CDLCLOSINGMARUBOZU', -0.074255704389433), ('2h_CDLSEPARATINGLINES', -0.08227851866376663), ('2h_CDLEVENINGSTAR', -0.08238535678322681), ('2h_CDLHOMINGPIGEON', 0.08264217907238317), ('2h_CDLSHOOTINGSTAR', -0.09208780177271089), ('2h_CDLADVANCEBLOCK', 0.09297138760692021), ('2h_CDLTRISTAR', -0.09387170783019683), ('2h_CDLCONCEALBABYSWALL', 0.09758183348504716), ('2h_CDL3LINESTRIKE', -0.10277753600488626), ('2h_CDLBREAKAWAY', -0.12278690620708829), ('12h_HT_PHASOR', 0.12503369133663547), ('2h_CDLHANGINGMAN', 0.12752582599097315), ('2h_CDL3INSIDE', 0.13143101581114003), ('2h_CDLCLOSINGMARUBOZU', -0.13506220698098825), ('12h_WILLR', 0.1351294605645096), ('12h_CDL3WHITESOLDIERS', 0.136109931954933), ('2h_CDLHIGHWAVE', 0.1381192464563186), ('12h_CDLADVANCEBLOCK', 0.14998396585134216), ('2h_CDLUNIQUE3RIVER', 0.1523513458674521), ('2h_CDL3WHITESOLDIERS', -0.15280504002741843), ('2h_CDLHAMMER', -0.1563517994210168), ('2h_TRIX', -0.1576057780301345), ('2h_AROONOSC', 0.1647961279542933), ('12h_CDLENGULFING', -0.16554454858387255), ('12h_CDL3OUTSIDE', -0.17142153987525469), ('12h_CDLHARAMI', 0.17379718998120366), ('12h_CDLMORNINGSTAR', -0.19488168001217787), ('2h_CDLONNECK', 0.1991446596954804), ('12h_CDLEVENINGSTAR', -0.2010751415187541), ('2h_CDLBELTHOLD', -0.20116265998259078), ('2h_CDLIDENTICAL3CROWS', -0.20468982146891002), ('2h_CDLDOJISTAR', 0.21237202299570163), ('2h_CDLLONGLEGGEDDOJI', 0.22873169564246323), ('2h_MFI', 0.22890591954759862), ('2h_CDLMATCHINGLOW', 0.23055667201067973), ('12h_CDLHARAMICROSS', -0.23868380636825892), ('2h_STOCH', -0.24394812410592065), ('2h_CDL2CROWS', 0.25215048109840554), ('2h_CDLMARUBOZU', 0.2612917070690703), ('12h_STOCH', -0.26226537243032516), ('12h_CDLTAKURI', 0.26245561759361535), ('12h_CDLHIKKAKEMOD', 0.27262559741567266), ('2h_CDLXSIDEGAP3METHODS', -0.27348961804492633), ('12h_CDLTRISTAR', 0.2745188839317273), ('12h_ULTOSC', -0.2997276128818435), ('12h_PPO2', 0.31428659491582467), ('12h_CDLDRAGONFLYDOJI', -0.3183363008961313), ('12h_CDLEVENINGDOJISTAR', -0.32192706400648596), ('12h_CDLINVERTEDHAMMER', -0.32485229642030033), ('2h_CDLPIERCING', 0.3251909906513806), ('12h_CDLGAPSIDESIDEWHITE', 0.32802059489866114), ('2h_CDLHARAMICROSS', 0.32867844760518705), ('2h_ADX', 0.34059103948781166), ('12h_CDLMORNINGDOJISTAR', -0.3634209813754601), ('2h_HT_DCPERIOD', 0.3657380833676169), ('2h_HT_DCPHASE', -0.3729983103784159), ('12h_CDLPIERCING', 0.38910052594286726), ('12h_CDLRICKSHAWMAN', 0.3953087643619167), ('2h_CDLMORNINGDOJISTAR', -0.3957687515947045), ('2h_CDLLONGLINE', -0.4091581649585763), ('12h_CDLHOMINGPIGEON', -0.414343927537707), ('12h_HT_DCPERIOD', 0.427751043677984), ('12h_CDLMATCHINGLOW', 0.4414583224379198), ('12h_CDLSHOOTINGSTAR', 0.47882703582497216), ('12h_CDLGRAVESTONEDOJI', 0.5561175295266274), ('2h_CDLSTALLEDPATTERN', -0.5595963816911543), ('12h_CDL2CROWS', 0.5682510708160035), ('2h_CDLHIKKAKEMOD', 0.5775160699692192), ('2h_CDLTHRUSTING', 0.5817345150643239), ('12h_CDLTASUKIGAP', -0.6100343679882801), ('2h_CDLRISEFALL3METHODS', -0.6424410595267579), ('2h_STOCHRSI', 0.6510805014500752), ('2h_PPO1', -0.6650483563291627), ('12h_CDLUNIQUE3RIVER', 0.7731707004654746), ('2h_CDLTASUKIGAP', -0.8272682237533966), ('12h_CMO', 0.8697940192867427), ('2h_PPO2', 0.9184841507912019), ('2h_STOCHF', -0.9873965143979972), ('12h_CCI', 1.1361434228560123), ('12h_PPO1', -1.1545716300558069), ('2h_CDL3BLACKCROWS', 1.1678274689819157), ('2h_CMO', -1.184695320525832), ('2h_RSI', -1.217982319019581), ('2h_WILLR', -1.2894636323011401), ('2h_ULTOSC', 1.6171715147861818), ('2h_CCI', 1.6759748000211567), ('2h_HT_PHASOR', 1.770966094776046)]</t>
+  </si>
+  <si>
+    <r>
+      <t>[('2h_CDLMATHOLD', 0.0), ('2h_CDLDOJI', 0.0), ('2h_CDLLADDERBOTTOM', 0.0), ('2h_CDLDRAGONFLYDOJI', 0.0), ('2h_CDLGRAVESTONEDOJI', 0.0), ('2h_CDLTAKURI', 0.0), ('2h_CDLENGULFING', 0.0), ('2h_CDLKICKING', 0.0), ('2h_CDLKICKINGBYLENGTH', 0.0), ('2h_HT_SINE', 0.0), ('2h_HT_TRENDMODE', 0.0), ('2h_CDL3OUTSIDE', 0.0), ('2h_CDLDARKCLOUDCOVER', 0.0), ('2h_DX', 0.0), ('2h_CDLMORNINGSTAR', 0.0), ('2h_CDLINNECK', 0.0), ('2h_CDLCOUNTERATTACK', 0.0), ('2h_CDL3STARSINSOUTH', 0.0), ('2h_CDLEVENINGDOJISTAR', 0.0), ('2h_CDLUPSIDEGAP2CROWS', 0.0), ('2h_CDLHARAMI', 0.0), ('2h_CDLABANDONEDBABY', 0.0), ('12h_RSI', 0.0), ('12h_CDLHIKKAKE', 0.0), ('12h_CDLMATHOLD', 0.0), ('12h_CDLBREAKAWAY', 0.0), ('12h_CDLDOJI', 0.0), ('12h_TRIX', 0.0), ('12h_CDLLADDERBOTTOM', 0.0), ('12h_CDLRISEFALL3METHODS', 0.0), ('12h_CDLHANGINGMAN', 0.0), ('12h_AROONOSC', 0.0), ('12h_MFI', 0.0), ('12h_CDLCONCEALBABYSWALL', 0.0), ('12h_CDLHAMMER', 0.0), ('12h_CDLLONGLINE', 0.0), ('12h_CDLLONGLEGGEDDOJI', 0.0), ('12h_CDL3LINESTRIKE', 0.0), ('12h_CDLSTALLEDPATTERN', 0.0), ('12h_CDLSHORTLINE', 0.0), ('12h_HT_DCPHASE', 0.0), ('12h_CDL3BLACKCROWS', 0.0), ('12h_CDLKICKING', 0.0), ('12h_CDLKICKINGBYLENGTH', 0.0), ('12h_HT_TRENDMODE', 0.0), ('12h_CDLIDENTICAL3CROWS', 0.0), ('12h_CDLDARKCLOUDCOVER', 0.0), ('12h_ADX', 0.0), ('12h_DX', 0.0), ('12h_CDLINNECK', 0.0), ('12h_CDLONNECK', 0.0), ('12h_CDLBELTHOLD', 0.0), ('12h_CDLCOUNTERATTACK', 0.0), ('12h_CDL3STARSINSOUTH', 0.0), ('12h_CDLUPSIDEGAP2CROWS', 0.0), ('12h_CDLTHRUSTING', 0.0), ('12h_CDLABANDONEDBABY', 0.0), ('12h_CDLHIGHWAVE', 0.0), ('12h_CDLSTICKSANDWICH', 0.0), ('12h_CDLSEPARATINGLINES', 0.003756276823238492), ('12h_HT_SINE', 0.009257156593133383), ('2h_CDLGAPSIDESIDEWHITE', -0.01386584544438379), ('2h_CDLSTICKSANDWICH', -0.01531186564737108), ('2h_CDLINVERTEDHAMMER', -0.030558377360614054), ('12h_CDLDOJISTAR', 0.033914071521249554), ('12h_STOCHF', 0.03519306895909331), ('12h_CDL3INSIDE', 0.03853514170349506), ('2h_CDLHIKKAKE', 0.04590047865208033), ('12h_CDLXSIDEGAP3METHODS', 0.05064224529817387), ('12h_CDLMARUBOZU'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF212121"/>
+        <rFont val="monospace"/>
+      </rPr>
+      <t>, 0.055460647430801126), ('12h_CDLSPINNINGTOP', -0.06041224990932476), ('2h_CDLRICKSHAWMAN', -0.06076636116761273), ('2h_CDLSPINNINGTOP', -0.06787611729649656), ('12h_STOCHRSI', -0.07045724225824293), ('2h_CDLSHORTLINE', -0.07404094923707907), ('12h_CDLCLOSINGMARUBOZU', -0.074255704389433), ('2h_CDLSEPARATINGLINES', -0.08227851866376663), ('2h_CDLEVENINGSTAR', -0.08238535678322681), ('2h_CDLHOMINGPIGEON', 0.08264217907238317), ('2h_CDLSHOOTINGSTAR', -0.09208780177271089), ('2h_CDLADVANCEBLOCK', 0.09297138760692021), ('2h_CDLTRISTAR', -0.09387170783019683), ('2h_CDLCONCEALBABYSWALL', 0.09758183348504716), ('2h_CDL3LINESTRIKE', -0.10277753600488626), ('2h_CDLBREAKAWAY', -0.12278690620708829), ('12h_HT_PHASOR', 0.12503369133663547), ('2h_CDLHANGINGMAN', 0.12752582599097315), ('2h_CDL3INSIDE', 0.13143101581114003), ('2h_CDLCLOSINGMARUBOZU', -0.13506220698098825), ('12h_WILLR', 0.1351294605645096), ('12h_CDL3WHITESOLDIERS', 0.136109931954933), ('2h_CDLHIGHWAVE', 0.1381192464563186), ('12h_CDLADVANCEBLOCK', 0.14998396585134216), ('2h_CDLUNIQUE3RIVER', 0.1523513458674521), ('2h_CDL3WHITESOLDIERS', -0.15280504002741843), ('2h_CDLHAMMER', -0.1563517994210168), ('2h_TRIX', -0.1576057780301345), ('2h_AROONOSC', 0.1647961279542933), ('12h_CDLENGULFING', -0.16554454858387255), ('12h_CDL3OUTSIDE', -0.17142153987525469), ('12h_CDLHARAMI', 0.17379718998120366), ('12h_CDLMORNINGSTAR', -0.19488168001217787), ('2h_CDLONNECK', 0.1991446596954804), ('12h_CDLEVENINGSTAR', -0.2010751415187541), ('2h_CDLBELTHOLD', -0.20116265998259078), ('2h_CDLIDENTICAL3CROWS', -0.20468982146891002), ('2h_CDLDOJISTAR', 0.21237202299570163), ('2h_CDLLONGLEGGEDDOJI', 0.22873169564246323), ('2h_MFI', 0.22890591954759862), ('2h_CDLMATCHINGLOW', 0.23055667201067973), ('12h_CDLHARAMICROSS', -0.23868380636825892), ('2h_STOCH', -0.24394812410592065), ('2h_CDL2CROWS', 0.25215048109840554), ('2h_CDLMARUBOZU', 0.2612917070690703), ('12h_STOCH', -0.26226537243032516), ('12h_CDLTAKURI', 0.26245561759361535), ('12h_CDLHIKKAKEMOD', 0.27262559741567266), ('2h_CDLXSIDE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF212121"/>
+        <rFont val="monospace"/>
+      </rPr>
+      <t>GAP3METHODS', -0.27348961804492633), ('12h_CDLTRISTAR', 0.2745188839317273), ('12h_ULTOSC', -0.2997276128818435), ('12h_PPO2', 0.31428659491582467), ('12h_CDLDRAGONFLYDOJI', -0.3183363008961313), ('12h_CDLEVENINGDOJISTAR', -0.32192706400648596), ('12h_CDLINVERTEDHAMMER', -0.32485229642030033), ('2h_CDLPIERCING', 0.3251909906513806), ('12h_CDLGAPSIDESIDEWHITE', 0.32802059489866114), ('2h_CDLHARAMICROSS', 0.32867844760518705), ('2h_ADX', 0.34059103948781166), ('12h_CDLMORNINGDOJISTAR', -0.3634209813754601), ('2h_HT_DCPERIOD', 0.3657380833676169), ('2h_HT_DCPHASE', -0.3729983103784159), ('12h_CDLPIERCING', 0.38910052594286726), ('12h_CDLRICKSHAWMAN', 0.3953087643619167), ('2h_CDLMORNINGDOJISTAR', -0.3957687515947045), ('2h_CDLLONGLINE', -0.4091581649585763), ('12h_CDLHOMINGPIGEON', -0.414343927537707), ('12h_HT_DCPERIOD', 0.427751043677984), ('12h_CDLMATCHINGLOW', 0.4414583224379198), ('12h_CDLSHOOTINGSTAR', 0.47882703582497216), ('12h_CDLGRAVESTONEDOJI', 0.5561175295266274), ('2h_CDLSTALLEDPATTERN', -0.5595963816911543), ('12h_CDL2CROWS', 0.5682510708160035), ('2h_CDLHIKKAKEMOD', 0.5775160699692192), ('2h_CDLTHRUSTING', 0.5817345150643239), ('12h_CDLTASUKIGAP', -0.6100343679882801), ('2h_CDLRISEFALL3METHODS', -0.6424410595267579), ('2h_STOCHRSI', 0.6510805014500752), ('2h_PPO1', -0.6650483563291627), ('12h_CDLUNIQUE3RIVER', 0.7731707004654746), ('2h_CDLTASUKIGAP', -0.8272682237533966), ('12h_CMO', 0.8697940192867427), ('2h_PPO2', 0.9184841507912019), ('2h_STOCHF', -0.9873965143979972), ('12h_CCI', 1.1361434228560123), ('12h_PPO1', -1.1545716300558069), ('2h_CDL3BLACKCROWS', 1.1678274689819157), ('2h_CMO', -1.184695320525832), ('2h_RSI', -1.217982319019581), ('2h_WILLR', -1.2894636323011401), ('2h_ULTOSC', 1.6171715147861818), ('2h_CCI', 1.6759748000211567), ('2h_HT_PHASOR', 1.770966094776046)]</t>
+    </r>
+  </si>
+  <si>
+    <t>[('2h_CDLMATHOLD', 0.0), ('2h_CDLBREAKAWAY', 0.0), ('2h_CDLDOJISTAR', 0.0), ('2h_CDLSHOOTINGSTAR', 0.0), ('2h_CDLHIKKAKEMOD', 0.0), ('2h_CDLLADDERBOTTOM', 0.0), ('2h_CDLRISEFALL3METHODS', 0.0), ('2h_CDLGRAVESTONEDOJI', 0.0), ('2h_CDLHANGINGMAN', 0.0), ('2h_CDLTASUKIGAP', 0.0), ('2h_CDLCONCEALBABYSWALL', 0.0), ('2h_CDLXSIDEGAP3METHODS', 0.0), ('2h_CDLINVERTEDHAMMER', 0.0), ('2h_CDLADVANCEBLOCK', 0.0), ('2h_CDL2CROWS', 0.0), ('2h_CDL3LINESTRIKE', 0.0), ('2h_CDLSTALLEDPATTERN', 0.0), ('2h_CDL3BLACKCROWS', 0.0), ('2h_CDLUNIQUE3RIVER', 0.0), ('2h_CDL3WHITESOLDIERS', 0.0), ('2h_CDLKICKING', 0.0), ('2h_CDLKICKINGBYLENGTH', 0.0), ('2h_CDLIDENTICAL3CROWS', 0.0), ('2h_CDLTRISTAR', 0.0), ('2h_CDL3OUTSIDE', 0.0), ('2h_CDLMATCHINGLOW', 0.0), ('2h_CDLGAPSIDESIDEWHITE', 0.0), ('2h_CDLDARKCLOUDCOVER', 0.0), ('2h_CDLMORNINGSTAR', 0.0), ('2h_CDL3INSIDE', 0.0), ('2h_CDLINNECK', 0.0), ('2h_CDLONNECK', 0.0), ('2h_CDLCOUNTERATTACK', 0.0), ('2h_CDLHARAMICROSS', 0.0), ('2h_CDL3STARSINSOUTH', 0.0), ('2h_CDLEVENINGDOJISTAR', 0.0), ('2h_CDLMORNINGDOJISTAR', 0.0), ('2h_CDLUPSIDEGAP2CROWS', 0.0), ('2h_CDLSEPARATINGLINES', 0.0), ('2h_CDLTHRUSTING', 0.0), ('2h_CDLHOMINGPIGEON', 0.0), ('2h_CDLPIERCING', 0.0), ('2h_CDLABANDONEDBABY', 0.0), ('2h_CDLEVENINGSTAR', 0.0), ('2h_CDLSTICKSANDWICH', 0.0), ('12h_CDLMATHOLD', 0.0), ('12h_CDLBREAKAWAY', 0.0), ('12h_CDLDOJISTAR', 0.0), ('12h_CDLSHOOTINGSTAR', 0.0), ('12h_CDLHIKKAKEMOD', 0.0), ('12h_CDLLADDERBOTTOM', 0.0), ('12h_CDLRISEFALL3METHODS', 0.0), ('12h_CDLGRAVESTONEDOJI', 0.0), ('12h_CDLTASUKIGAP', 0.0), ('12h_CDLCONCEALBABYSWALL', 0.0), ('12h_CDLXSIDEGAP3METHODS', 0.0), ('12h_CDLHAMMER', 0.0), ('12h_CDLINVERTEDHAMMER', 0.0), ('12h_CDLADVANCEBLOCK', 0.0), ('12h_CDL2CROWS', 0.0), ('12h_CDL3LINESTRIKE', 0.0), ('12h_CDLSTALLEDPATTERN', 0.0), ('12h_CDLTAKURI', 0.0), ('12h_CDL3BLACKCROWS', 0.0), ('12h_CDLUNIQUE3RIVER', 0.0), ('12h_CDL3WHITESOLDIERS', 0.0), ('12h_CDLENGULFING', 0.0), ('12h_CDLKICKING', 0.0), ('12h_CDLKICKINGBYLENGTH', 0.0), ('12h_CDLIDENTICAL3CROWS', 0.0), ('12h_CDLTRISTAR', 0.0), ('12h_CDL3OUTSIDE', 0.0), ('12h_CDLMATCHINGLOW', 0.0), ('12h_CDLGAPSIDESIDEWHITE', 0.0), ('12h_CDLDARKCLOUDCOVER', 0.0), ('12h_CDLMORNINGSTAR', 0.0), ('12h_CDL3INSIDE', 0.0), ('12h_CDLINNECK', 0.0), ('12h_CDLONNECK', 0.0), ('12h_CDLCOUNTERATTACK', 0.0), ('12h_CDLHARAMICROSS', 0.0), ('12h_CDL3STARSINSOUTH', 0.0), ('12h_CDLEVENINGDOJISTAR', 0.0), ('12h_CDLMORNINGDOJISTAR', 0.0), ('12h_CDLUPSIDEGAP2CROWS', 0.0), ('12h_CDLSEPARATINGLINES', 0.0), ('12h_CDLTHRUSTING', 0.0), ('12h_CDLHOMINGPIGEON', 0.0), ('12h_CDLPIERCING', 0.0), ('12h_CDLABANDONEDBABY', 0.0), ('12h_CDLEVENINGSTAR', 0.0), ('12h_CDLSTICKSANDWICH', 0.0), ('12h_CDLDRAGONFLYDOJI', 3.518012812909512e-05), ('2h_CDLTAKURI', 9.580125412890372e-05), ('12h_CDLHANGINGMAN', 0.0001468801726882232), ('2h_CDLDRAGONFLYDOJI', 0.0001617033625283365), ('12h_CDLHARAMI', 0.0002115003809572444), ('12h_CDLHIGHWAVE', 0.0002187553999055074), ('12h_CDLMARUBOZU', 0.00022827024639948017), ('2h_CDLHAMMER', 0.00030258129939067215), ('12h_CDLCLOSINGMARUBOZU', 0.0004288232255992445), ('2h_CDLRICKSHAWMAN', 0.0004620246446382284), ('2h_CDLHARAMI', 0.00051373757922485), ('12h_CDLSPINNINGTOP', 0.0005219023923823332), ('2h_CDLHIGHWAVE', 0.000637526737622254), ('2h_CDLLONGLEGGEDDOJI', 0.0006498048298774242), ('12h_CDLLONGLEGGEDDOJI', 0.0006611568239867864), ('12h_HT_TRENDMODE', 0.0007084979512787184), ('12h_CDLLONGLINE', 0.0007146772518008718), ('12h_CDLRICKSHAWMAN', 0.0007711206418534955), ('2h_CDLENGULFING', 0.0009959193135586901), ('2h_CDLSPINNINGTOP', 0.0011119129509835075), ('2h_CDLDOJI', 0.0011961986306134118), ('12h_CDLHIKKAKE', 0.0012657499223417226), ('12h_CDLDOJI', 0.0013392149664783418), ('12h_CDLBELTHOLD', 0.0015052635206983822), ('12h_CDLSHORTLINE', 0.0016481563839429744), ('2h_CDLSHORTLINE', 0.0016905746869643754), ('2h_CDLHIKKAKE', 0.0019423355089722087), ('2h_CDLMARUBOZU', 0.0031294335821718472), ('2h_HT_TRENDMODE', 0.004660846299509167), ('2h_CDLLONGLINE', 0.007061793382313584), ('2h_CDLCLOSINGMARUBOZU', 0.009467846263767968), ('12h_AROONOSC', 0.011274616922037836), ('12h_HT_PHASOR', 0.01453925757417426), ('2h_CDLBELTHOLD', 0.015860810115229208), ('12h_ADX', 0.016203383738903013), ('12h_STOCHF', 0.016511767099188196), ('2h_AROONOSC', 0.016908061291068015), ('2h_DX', 0.01803200656689309), ('12h_STOCHRSI', 0.019238077601045317), ('2h_ADX', 0.020111976979412267), ('12h_STOCH', 0.020140574965023195), ('12h_DX', 0.020175840105282453), ('2h_PPO1', 0.02066708156467577), ('12h_WILLR', 0.020795609081532315), ('12h_HT_DCPERIOD', 0.02193830424419609), ('12h_HT_SINE', 0.02299586760874611), ('12h_PPO1', 0.023709791852057842), ('12h_MFI', 0.023805928918557717), ('12h_HT_DCPHASE', 0.024139527918426246), ('12h_ULTOSC', 0.0248407221451051), ('12h_CCI', 0.02489376293042076), ('2h_CCI', 0.025169240791544784), ('2h_TRIX', 0.025615212799137203), ('2h_MFI', 0.0257899889946091), ('2h_ULTOSC', 0.026231345690333495), ('2h_RSI', 0.026435036813157266), ('2h_HT_DCPERIOD', 0.026704565860606103), ('2h_HT_DCPHASE', 0.027146120558799076), ('2h_CMO', 0.027416145359273343), ('2h_PPO2', 0.027419992819313874), ('12h_CMO', 0.028032508293940425), ('12h_PPO2', 0.02822661828188017), ('2h_STOCHRSI', 0.02833109695704975), ('2h_HT_SINE', 0.028432282881418906), ('12h_RSI', 0.029731494849986814), ('2h_HT_PHASOR', 0.03084594654547924), ('12h_TRIX', 0.03149020505978931), ('2h_STOCH', 0.03200496016540793), ('2h_WILLR', 0.03902513621516563), ('2h_STOCHF', 0.044683942106425005)]</t>
+  </si>
+  <si>
+    <t>SGDClassifier</t>
+  </si>
+  <si>
+    <t>RandomForestClassifier</t>
+  </si>
+  <si>
+    <t>LinearSVC</t>
+  </si>
+  <si>
+    <t>[('2h_CDLMATHOLD', 0.0), ('2h_CDLKICKING', 0.0), ('2h_CDLKICKINGBYLENGTH', 0.0), ('2h_CDLCOUNTERATTACK', 0.0), ('2h_CDL3STARSINSOUTH', 0.0), ('2h_CDLUPSIDEGAP2CROWS', 0.0), ('2h_CDLABANDONEDBABY', 0.0), ('12h_CDLMATHOLD', 0.0), ('12h_CDLBREAKAWAY', 0.0), ('12h_CDLLADDERBOTTOM', 0.0), ('12h_CDLCONCEALBABYSWALL', 0.0), ('12h_CDL3BLACKCROWS', 0.0), ('12h_CDLKICKING', 0.0), ('12h_CDLKICKINGBYLENGTH', 0.0), ('12h_CDLIDENTICAL3CROWS', 0.0), ('12h_CDLINNECK', 0.0), ('12h_CDLONNECK', 0.0), ('12h_CDLCOUNTERATTACK', 0.0), ('12h_CDL3STARSINSOUTH', 0.0), ('12h_CDLUPSIDEGAP2CROWS', 0.0), ('12h_CDLABANDONEDBABY', 0.0), ('12h_CDLDOJISTAR', 0.0007051941056163136), ('2h_HT_TRENDMODE', -0.00129857795600552), ('2h_CDLEVENINGSTAR', 0.0013371376004388535), ('2h_CDLGRAVESTONEDOJI', 0.0019070132642409199), ('12h_AROONOSC', -0.0020821099430312928), ('12h_MFI', -0.002446253257620162), ('12h_CDLXSIDEGAP3METHODS', 0.002902839595455786), ('2h_HT_SINE', -0.002979713423727426), ('12h_HT_SINE', 0.00324508094207634), ('2h_CDL3OUTSIDE', 0.005104129885975972), ('12h_CDLSTALLEDPATTERN', -0.005504238746958379), ('12h_HT_TRENDMODE', 0.0057217675997346396), ('12h_RSI', 0.007111135210351718), ('12h_DX', 0.010016445203791961), ('12h_ADX', -0.010345274476403257), ('12h_CDLCLOSINGMARUBOZU', -0.010486014767880192), ('12h_CDLHIGHWAVE', 0.010498403046730664), ('12h_CDLLONGLINE', -0.011753163206750794), ('2h_DX', -0.014241662248544442), ('12h_CDLHARAMI', 0.0153098120065992), ('12h_CDLHAMMER', -0.01570061209526763), ('12h_CDLENGULFING', -0.016040986093552534), ('12h_CDLHIKKAKE', 0.016457542221978372), ('2h_CDLENGULFING', 0.016493739834726684), ('12h_CDLBELTHOLD', -0.018222856194564208), ('12h_CDLSPINNINGTOP', -0.018696924874180954), ('12h_CDLSHORTLINE', 0.019124350646726795), ('2h_CDLDARKCLOUDCOVER', 0.019251559804928986), ('12h_CDL3LINESTRIKE', 0.019752868099607857), ('12h_HT_DCPHASE', 0.02043218717224268), ('12h_CDLHANGINGMAN', 0.02101935055787485), ('2h_CDLHANGINGMAN', 0.02175988989137867), ('2h_CDLHARAMI', -0.02256120582750165), ('2h_CDLSHOOTINGSTAR', -0.022950155505864545), ('2h_CDLSEPARATINGLINES', -0.02357750045327589), ('2h_CDLDOJISTAR', 0.02481419173498456), ('12h_STOCH', -0.02502041294992493), ('2h_CDLINVERTEDHAMMER', -0.025620606636932886), ('2h_CDLTAKURI', -0.025947323183245552), ('2h_CDLSHORTLINE', -0.026222009668070312), ('12h_CDL3INSIDE', 0.026538773090108436), ('12h_CDLSEPARATINGLINES', 0.027128807888476603), ('2h_AROONOSC', 0.027658655361860626), ('2h_CDLDOJI', -0.02928538829563021), ('12h_CDLDARKCLOUDCOVER', -0.029687173578781867), ('2h_CDLDRAGONFLYDOJI', 0.0299611986223991), ('12h_CDLADVANCEBLOCK', 0.03026150651352766), ('12h_CDLTHRUSTING', 0.030458257422112056), ('12h_CDLMORNINGSTAR', -0.03049429880761273), ('12h_WILLR', 0.031757704840890716), ('2h_CDLHIGHWAVE', 0.03408086959471146), ('2h_CDLCLOSINGMARUBOZU', -0.03469405675879178), ('12h_CDLLONGLEGGEDDOJI', -0.0365866562881757), ('2h_STOCH', -0.0370450896745343), ('12h_STOCHRSI', -0.039624439892627886), ('2h_CDLGAPSIDESIDEWHITE', -0.04148826554493834), ('2h_CDL3WHITESOLDIERS', -0.04806949935790972), ('2h_CDLLONGLINE', -0.04827823296571088), ('2h_CDLHAMMER', -0.048454072535241366), ('2h_CDLSPINNINGTOP', -0.05029365598944924), ('2h_CDLSTICKSANDWICH', -0.05105450213512275), ('2h_CDLXSIDEGAP3METHODS', -0.05119500958291201), ('12h_CDL3OUTSIDE', -0.05178432228049368), ('2h_CDLHIKKAKE', 0.05383797219186509), ('2h_CDLHARAMICROSS', 0.054237132622378836), ('2h_CDLEVENINGDOJISTAR', 0.055217457622934174), ('12h_CDLMARUBOZU', 0.0580389150827918), ('2h_CDLADVANCEBLOCK', 0.05904940209797349), ('2h_CDL3INSIDE', 0.060329770720871645), ('2h_CDLRICKSHAWMAN', -0.0603532638983969), ('12h_CDLDOJI', -0.06151751970357544), ('12h_CDLEVENINGSTAR', -0.06644112581101558), ('2h_HT_DCPHASE', -0.06673224125831884), ('2h_CDLLONGLEGGEDDOJI', 0.06894379161226871), ('2h_CDLMARUBOZU', 0.07042402554090627), ('12h_CDLHARAMICROSS', -0.0731609556622107), ('12h_CDLRICKSHAWMAN', 0.07413266863370005), ('2h_CDLBELTHOLD', -0.07746552786974037), ('12h_CDL3WHITESOLDIERS', 0.07837925616197733), ('2h_CDLTRISTAR', -0.07952908466628261), ('2h_CMO', -0.08025409566842104), ('2h_CDL3LINESTRIKE', -0.08132066709033725), ('12h_CDLDRAGONFLYDOJI', -0.08430449980023369), ('2h_ADX', 0.09043647635515452), ('2h_CDLHOMINGPIGEON', 0.09401754055461231), ('2h_MFI', 0.09770716637898755), ('2h_CDLMORNINGSTAR', 0.0990500858994795), ('12h_CDLINVERTEDHAMMER', -0.10357983015136785), ('12h_ULTOSC', -0.10559154881062377), ('12h_CDLGAPSIDESIDEWHITE', 0.11183795269555807), ('2h_CDLMATCHINGLOW', 0.11572824019916528), ('12h_CDLTAKURI', 0.11730815283091378), ('12h_HT_PHASOR', 0.11797772977449915), ('12h_CDLSTICKSANDWICH', -0.11799755326674172), ('12h_CDLMATCHINGLOW', 0.1185803291344163), ('2h_CDLPIERCING', 0.12066501225706205), ('12h_CDLMORNINGDOJISTAR', -0.1254854062226981), ('12h_HT_DCPERIOD', 0.12836652370801752), ('12h_STOCHF', 0.13139349347404977), ('12h_CDLHIKKAKEMOD', 0.13473721654120907), ('2h_HT_DCPERIOD', 0.141631434695155), ('12h_PPO2', 0.14198419906120643), ('2h_CDLLADDERBOTTOM', 0.14580794288877463), ('12h_CDLSHOOTINGSTAR', 0.15016014341837713), ('2h_CDL2CROWS', 0.15232116214077873), ('12h_CDLEVENINGDOJISTAR', -0.15806359366681777), ('12h_CDLGRAVESTONEDOJI', 0.1602713367006401), ('2h_CDLTHRUSTING', 0.17253990952242038), ('2h_CDLUNIQUE3RIVER', 0.17878520393456426), ('12h_CDLTRISTAR', 0.18761263321244392), ('12h_CDLHOMINGPIGEON', -0.1950158770942917), ('2h_CDLSTALLEDPATTERN', -0.19833328138565098), ('2h_CDLONNECK', 0.20644966266793818), ('2h_STOCHRSI', 0.20765546616946126), ('12h_CDLRISEFALL3METHODS', 0.21023729104572908), ('2h_CDLINNECK', -0.23546930742799077), ('2h_CDLMORNINGDOJISTAR', -0.2428623761626988), ('2h_STOCHF', -0.24694312389456502), ('2h_CDLIDENTICAL3CROWS', -0.24828816618851046), ('2h_CDLHIKKAKEMOD', 0.25604191442276336), ('12h_CDL2CROWS', 0.3016389431767149), ('12h_CMO', 0.3473719756461872), ('12h_CDLTASUKIGAP', -0.36708228372918084), ('2h_CDLTASUKIGAP', -0.36715239251266674), ('2h_WILLR', -0.38667722227804413), ('12h_CDLPIERCING', 0.4540149251047687), ('12h_TRIX', -0.47791356544584057), ('2h_CDLRISEFALL3METHODS', -0.5140303640950318), ('12h_CCI', 0.5511427773670614), ('12h_CDLUNIQUE3RIVER', 0.573642843688891), ('2h_CDLCONCEALBABYSWALL', 0.594378769557557), ('2h_ULTOSC', 0.6132862338137712), ('2h_PPO2', 0.6532692719156086), ('2h_TRIX', 0.7637428672489253), ('2h_CCI', 0.8205073418495358), ('2h_PPO1', -0.8500048262454559), ('2h_CDL3BLACKCROWS', 0.8882906846652598), ('2h_CDLBREAKAWAY', -0.9361260045596477), ('12h_PPO1', -0.959369139235711), ('2h_RSI', -1.1792385198683581), ('2h_HT_PHASOR', 2.0186146217621164)]</t>
+  </si>
+  <si>
+    <t>XGBClassifier</t>
+  </si>
+  <si>
+    <t>[('2h_CDLMATHOLD', 0.0), ('2h_CDLBREAKAWAY', 0.0), ('2h_CDLDOJISTAR', 0.0), ('2h_CDLHIKKAKEMOD', 0.0), ('2h_CDLLADDERBOTTOM', 0.0), ('2h_CDLRISEFALL3METHODS', 0.0), ('2h_CDLCONCEALBABYSWALL', 0.0), ('2h_CDL2CROWS', 0.0), ('2h_CDL3LINESTRIKE', 0.0), ('2h_CDL3BLACKCROWS', 0.0), ('2h_CDLUNIQUE3RIVER', 0.0), ('2h_CDLKICKING', 0.0), ('2h_CDLKICKINGBYLENGTH', 0.0), ('2h_CDLIDENTICAL3CROWS', 0.0), ('2h_CDLTRISTAR', 0.0), ('2h_CDLGAPSIDESIDEWHITE', 0.0), ('2h_CDLDARKCLOUDCOVER', 0.0), ('2h_CDLMORNINGSTAR', 0.0), ('2h_CDLINNECK', 0.0), ('2h_CDLONNECK', 0.0), ('2h_CDLCOUNTERATTACK', 0.0), ('2h_CDL3STARSINSOUTH', 0.0), ('2h_CDLEVENINGDOJISTAR', 0.0), ('2h_CDLMORNINGDOJISTAR', 0.0), ('2h_CDLUPSIDEGAP2CROWS', 0.0), ('2h_CDLHOMINGPIGEON', 0.0), ('2h_CDLPIERCING', 0.0), ('2h_CDLABANDONEDBABY', 0.0), ('2h_CDLSTICKSANDWICH', 0.0), ('12h_CDLMATHOLD', 0.0), ('12h_CDLBREAKAWAY', 0.0), ('12h_CDLHIKKAKEMOD', 0.0), ('12h_CDLLADDERBOTTOM', 0.0), ('12h_CDLRISEFALL3METHODS', 0.0), ('12h_CDLTASUKIGAP', 0.0), ('12h_CDLCONCEALBABYSWALL', 0.0), ('12h_CDLINVERTEDHAMMER', 0.0), ('12h_CDL2CROWS', 0.0), ('12h_CDL3LINESTRIKE', 0.0), ('12h_CDLSTALLEDPATTERN', 0.0), ('12h_CDL3BLACKCROWS', 0.0), ('12h_CDLUNIQUE3RIVER', 0.0), ('12h_CDL3WHITESOLDIERS', 0.0), ('12h_CDLKICKING', 0.0), ('12h_CDLKICKINGBYLENGTH', 0.0), ('12h_CDLIDENTICAL3CROWS', 0.0), ('12h_CDLTRISTAR', 0.0), ('12h_CDLGAPSIDESIDEWHITE', 0.0), ('12h_CDLMORNINGSTAR', 0.0), ('12h_CDLINNECK', 0.0), ('12h_CDLONNECK', 0.0), ('12h_CDLCOUNTERATTACK', 0.0), ('12h_CDL3STARSINSOUTH', 0.0), ('12h_CDLEVENINGDOJISTAR', 0.0), ('12h_CDLMORNINGDOJISTAR', 0.0), ('12h_CDLUPSIDEGAP2CROWS', 0.0), ('12h_CDLTHRUSTING', 0.0), ('12h_CDLHOMINGPIGEON', 0.0), ('12h_CDLPIERCING', 0.0), ('12h_CDLABANDONEDBABY', 0.0), ('12h_CDLEVENINGSTAR', 0.0), ('12h_CDLSTICKSANDWICH', 0.0), ('2h_CDLHARAMICROSS', 0.0017391085), ('2h_CDLXSIDEGAP3METHODS', 0.0026703614), ('2h_CDL3WHITESOLDIERS', 0.0049547385), ('12h_CDLHARAMICROSS', 0.006116293), ('12h_HT_TRENDMODE', 0.0061506913), ('12h_CDLGRAVESTONEDOJI', 0.006718129), ('2h_HT_DCPERIOD', 0.006744384), ('2h_CDLTHRUSTING', 0.0068080905), ('2h_CDL3INSIDE', 0.006844308), ('12h_DX', 0.0068921284), ('2h_CDLTASUKIGAP', 0.0070326924), ('12h_ADX', 0.0070992648), ('12h_HT_DCPHASE', 0.0073046223), ('12h_CDLHAMMER', 0.0073308605), ('12h_CDL3INSIDE', 0.0074531767), ('12h_WILLR', 0.007454603), ('2h_CMO', 0.007484344), ('12h_PPO1', 0.007510935), ('12h_CDLLONGLEGGEDDOJI', 0.0075140037), ('2h_PPO2', 0.007524774), ('12h_RSI', 0.0076096873), ('2h_ADX', 0.0076750712), ('12h_CCI', 0.007745791), ('12h_CDLDRAGONFLYDOJI', 0.007746291), ('12h_HT_SINE', 0.007758133), ('12h_STOCHF', 0.007826242), ('12h_CDLBELTHOLD', 0.007834388), ('2h_CDLMATCHINGLOW', 0.007864183), ('12h_TRIX', 0.007912021), ('2h_STOCHF', 0.007925613), ('12h_HT_PHASOR', 0.007961343), ('2h_MFI', 0.007967982), ('12h_ULTOSC', 0.007985881), ('12h_PPO2', 0.008015514), ('2h_WILLR', 0.008030714), ('12h_CDLLONGLINE', 0.008055876), ('2h_HT_SINE', 0.008155716), ('2h_ULTOSC', 0.008169167), ('2h_DX', 0.008172688), ('2h_STOCHRSI', 0.008172868), ('2h_HT_DCPHASE', 0.008253407), ('12h_AROONOSC', 0.00837656), ('2h_AROONOSC', 0.008447013), ('12h_HT_DCPERIOD', 0.008499744), ('2h_PPO1', 0.008515037), ('2h_STOCH', 0.008561264), ('12h_MFI', 0.008597082), ('2h_TRIX', 0.008598709), ('12h_STOCH', 0.008719588), ('12h_STOCHRSI', 0.008735583), ('2h_HT_TRENDMODE', 0.008811087), ('12h_CDLRICKSHAWMAN', 0.008826421), ('2h_HT_PHASOR', 0.008927663), ('12h_CDLMATCHINGLOW', 0.00896993), ('2h_CCI', 0.009172719), ('2h_CDLHARAMI', 0.009187829), ('12h_CDLMARUBOZU', 0.009399981), ('12h_CMO', 0.009647711), ('2h_CDLSHORTLINE', 0.009753032), ('2h_CDLENGULFING', 0.0097931335), ('2h_CDLCLOSINGMARUBOZU', 0.009877941), ('12h_CDLDOJI', 0.009880465), ('12h_CDLHIKKAKE', 0.009975562), ('2h_CDLHIGHWAVE', 0.009976349), ('12h_CDLCLOSINGMARUBOZU', 0.010098745), ('12h_CDLSPINNINGTOP', 0.01028659), ('12h_CDLDARKCLOUDCOVER', 0.010299606), ('12h_CDLSHORTLINE', 0.010336074), ('2h_CDLRICKSHAWMAN', 0.010392776), ('2h_CDLHIKKAKE', 0.010439168), ('2h_CDLDOJI', 0.010553823), ('2h_CDLHANGINGMAN', 0.01057511), ('12h_CDL3OUTSIDE', 0.0106982), ('2h_CDLGRAVESTONEDOJI', 0.010865725), ('12h_CDLHIGHWAVE', 0.010880766), ('12h_CDLHARAMI', 0.011367543), ('2h_CDLDRAGONFLYDOJI', 0.011402754), ('2h_CDLHAMMER', 0.011561077), ('12h_CDLENGULFING', 0.011614598), ('2h_RSI', 0.01169088), ('2h_CDLLONGLEGGEDDOJI', 0.01212931), ('12h_CDLADVANCEBLOCK', 0.01279526), ('2h_CDLSTALLEDPATTERN', 0.0129304305), ('2h_CDLMARUBOZU', 0.013113995), ('12h_CDLTAKURI', 0.013276949), ('12h_CDLSHOOTINGSTAR', 0.013508402), ('2h_CDLSPINNINGTOP', 0.013724369), ('12h_CDLXSIDEGAP3METHODS', 0.014061773), ('2h_CDLSEPARATINGLINES', 0.014540767), ('2h_CDL3OUTSIDE', 0.014554604), ('2h_CDLLONGLINE', 0.0150164105), ('2h_CDLTAKURI', 0.015505098), ('12h_CDLHANGINGMAN', 0.016567245), ('2h_CDLADVANCEBLOCK', 0.016685594), ('2h_CDLINVERTEDHAMMER', 0.017416788), ('2h_CDLSHOOTINGSTAR', 0.017783737), ('2h_CDLBELTHOLD', 0.019352026), ('12h_CDLDOJISTAR', 0.019794088), ('12h_CDLSEPARATINGLINES', 0.019986678), ('2h_CDLEVENINGSTAR', 0.028756559)]</t>
+  </si>
+  <si>
+    <t>MLPClassifier</t>
+  </si>
+  <si>
+    <r>
+      <t>[('2h_CDLMATHOLD', 0.0), ('2h_CDLDOJI', 0.0), ('2h_CDLLADDERBOTTOM', 0.0), ('2h_CDLDRAGONFLYDOJI', 0.0), ('2h_CDLGRAVESTONEDOJI', 0.0), ('2h_CDLTAKURI', 0.0), ('2h_CDLENGULFING', 0.0), ('2h_CDLKICKING', 0.0), ('2h_CDLKICKINGBYLENGTH', 0.0), ('2h_HT_SINE', 0.0), ('2h_HT_TRENDMODE', 0.0), ('2h_CDL3OUTSIDE', 0.0), ('2h_CDLDARKCLOUDCOVER', 0.0), ('2h_DX', 0.0), ('2h_CDLMORNINGSTAR', 0.0), ('2h_CDLINNECK', 0.0), ('2h_CDLCOUNTERATTACK', 0.0), ('2h_CDL3STARSINSOUTH', 0.0), ('2h_CDLEVENINGDOJISTAR', 0.0), ('2h_CDLUPSIDEGAP2CROWS', 0.0), ('2h_CDLHARAMI', 0.0), ('2h_CDLABANDONEDBABY', 0.0), ('12h_RSI', 0.0), ('12h_CDLHIKKAKE', 0.0), ('12h_CDLMATHOLD', 0.0), ('12h_CDLBREAKAWAY', 0.0), ('12h_CDLDOJI', 0.0), ('12h_TRIX', 0.0), ('12h_CDLLADDERBOTTOM', 0.0), ('12h_CDLRISEFALL3METHODS', 0.0), ('12h_CDLHANGINGMAN', 0.0), ('12h_AROONOSC', 0.0), ('12h_MFI', 0.0), ('12h_CDLCONCEALBABYSWALL', 0.0), ('12h_CDLHAMMER', 0.0), ('12h_CDLLONGLINE', 0.0), ('12h_CDLLONGLEGGEDDOJI', 0.0), ('12h_CDL3LINESTRIKE', 0.0), ('12h_CDLSTALLEDPATTERN', 0.0), ('12h_CDLSHORTLINE', 0.0), ('12h_HT_DCPHASE', 0.0), ('12h_CDL3BLACKCROWS', 0.0), ('12h_CDLKICKING', 0.0), ('12h_CDLKICKINGBYLENGTH', 0.0), ('12h_HT_TRENDMODE', 0.0), ('12h_CDLIDENTICAL3CROWS', 0.0), ('12h_CDLDARKCLOUDCOVER', 0.0), ('12h_ADX', 0.0), ('12h_DX', 0.0), ('12h_CDLINNECK', 0.0), ('12h_CDLONNECK', 0.0), ('12h_CDLBELTHOLD', 0.0), ('12h_CDLCOUNTERATTACK', 0.0), ('12h_CDL3STARSINSOUTH', 0.0), ('12h_CDLUPSIDEGAP2CROWS', 0.0), ('12h_CDLTHRUSTING', 0.0), ('12h_CDLABANDONEDBABY', 0.0), ('12h_CDLHIGHWAVE', 0.0), ('12h_CDLSTICKSANDWICH', 0.0), ('12h_CDLSEPARATINGLINES', 0.003756276823238492), ('12h_HT_SINE', 0.009257156593133383), ('2h_CDLGAPSIDESIDEWHITE', -0.01386584544438379), ('2h_CDLSTICKSANDWICH', -0.01531186564737108), ('2h_CDLINVERTEDHAMMER', -0.030558377360614054), ('12h_CDLDOJISTAR', 0.033914071521249554), ('12h_STOCHF', 0.03519306895909331), ('12h_CDL3INSIDE', 0.03853514170349506), ('2h_CDLHIKKAKE', 0.04590047865208033), ('12h_CDLXSIDEGAP3METHODS', 0.05064224529817387), ('12h_CDLMARUBOZU'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="monospace"/>
+      </rPr>
+      <t>, 0.055460647430801126), ('12h_CDLSPINNINGTOP', -0.06041224990932476), ('2h_CDLRICKSHAWMAN', -0.06076636116761273), ('2h_CDLSPINNINGTOP', -0.06787611729649656), ('12h_STOCHRSI', -0.07045724225824293), ('2h_CDLSHORTLINE', -0.07404094923707907), ('12h_CDLCLOSINGMARUBOZU', -0.074255704389433), ('2h_CDLSEPARATINGLINES', -0.08227851866376663), ('2h_CDLEVENINGSTAR', -0.08238535678322681), ('2h_CDLHOMINGPIGEON', 0.08264217907238317), ('2h_CDLSHOOTINGSTAR', -0.09208780177271089), ('2h_CDLADVANCEBLOCK', 0.09297138760692021), ('2h_CDLTRISTAR', -0.09387170783019683), ('2h_CDLCONCEALBABYSWALL', 0.09758183348504716), ('2h_CDL3LINESTRIKE', -0.10277753600488626), ('2h_CDLBREAKAWAY', -0.12278690620708829), ('12h_HT_PHASOR', 0.12503369133663547), ('2h_CDLHANGINGMAN', 0.12752582599097315), ('2h_CDL3INSIDE', 0.13143101581114003), ('2h_CDLCLOSINGMARUBOZU', -0.13506220698098825), ('12h_WILLR', 0.1351294605645096), ('12h_CDL3WHITESOLDIERS', 0.136109931954933), ('2h_CDLHIGHWAVE', 0.1381192464563186), ('12h_CDLADVANCEBLOCK', 0.14998396585134216), ('2h_CDLUNIQUE3RIVER', 0.1523513458674521), ('2h_CDL3WHITESOLDIERS', -0.15280504002741843), ('2h_CDLHAMMER', -0.1563517994210168), ('2h_TRIX', -0.1576057780301345), ('2h_AROONOSC', 0.1647961279542933), ('12h_CDLENGULFING', -0.16554454858387255), ('12h_CDL3OUTSIDE', -0.17142153987525469), ('12h_CDLHARAMI', 0.17379718998120366), ('12h_CDLMORNINGSTAR', -0.19488168001217787), ('2h_CDLONNECK', 0.1991446596954804), ('12h_CDLEVENINGSTAR', -0.2010751415187541), ('2h_CDLBELTHOLD', -0.20116265998259078), ('2h_CDLIDENTICAL3CROWS', -0.20468982146891002), ('2h_CDLDOJISTAR', 0.21237202299570163), ('2h_CDLLONGLEGGEDDOJI', 0.22873169564246323), ('2h_MFI', 0.22890591954759862), ('2h_CDLMATCHINGLOW', 0.23055667201067973), ('12h_CDLHARAMICROSS', -0.23868380636825892), ('2h_STOCH', -0.24394812410592065), ('2h_CDL2CROWS', 0.25215048109840554), ('2h_CDLMARUBOZU', 0.2612917070690703), ('12h_STOCH', -0.26226537243032516), ('12h_CDLTAKURI', 0.26245561759361535), ('12h_CDLHIKKAKEMOD', 0.27262559741567266), ('2h_CDLXSIDE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="monospace"/>
+      </rPr>
+      <t>GAP3METHODS', -0.27348961804492633), ('12h_CDLTRISTAR', 0.2745188839317273), ('12h_ULTOSC', -0.2997276128818435), ('12h_PPO2', 0.31428659491582467), ('12h_CDLDRAGONFLYDOJI', -0.3183363008961313), ('12h_CDLEVENINGDOJISTAR', -0.32192706400648596), ('12h_CDLINVERTEDHAMMER', -0.32485229642030033), ('2h_CDLPIERCING', 0.3251909906513806), ('12h_CDLGAPSIDESIDEWHITE', 0.32802059489866114), ('2h_CDLHARAMICROSS', 0.32867844760518705), ('2h_ADX', 0.34059103948781166), ('12h_CDLMORNINGDOJISTAR', -0.3634209813754601), ('2h_HT_DCPERIOD', 0.3657380833676169), ('2h_HT_DCPHASE', -0.3729983103784159), ('12h_CDLPIERCING', 0.38910052594286726), ('12h_CDLRICKSHAWMAN', 0.3953087643619167), ('2h_CDLMORNINGDOJISTAR', -0.3957687515947045), ('2h_CDLLONGLINE', -0.4091581649585763), ('12h_CDLHOMINGPIGEON', -0.414343927537707), ('12h_HT_DCPERIOD', 0.427751043677984), ('12h_CDLMATCHINGLOW', 0.4414583224379198), ('12h_CDLSHOOTINGSTAR', 0.47882703582497216), ('12h_CDLGRAVESTONEDOJI', 0.5561175295266274), ('2h_CDLSTALLEDPATTERN', -0.5595963816911543), ('12h_CDL2CROWS', 0.5682510708160035), ('2h_CDLHIKKAKEMOD', 0.5775160699692192), ('2h_CDLTHRUSTING', 0.5817345150643239), ('12h_CDLTASUKIGAP', -0.6100343679882801), ('2h_CDLRISEFALL3METHODS', -0.6424410595267579), ('2h_STOCHRSI', 0.6510805014500752), ('2h_PPO1', -0.6650483563291627), ('12h_CDLUNIQUE3RIVER', 0.7731707004654746), ('2h_CDLTASUKIGAP', -0.8272682237533966), ('12h_CMO', 0.8697940192867427), ('2h_PPO2', 0.9184841507912019), ('2h_STOCHF', -0.9873965143979972), ('12h_CCI', 1.1361434228560123), ('12h_PPO1', -1.1545716300558069), ('2h_CDL3BLACKCROWS', 1.1678274689819157), ('2h_CMO', -1.184695320525832), ('2h_RSI', -1.217982319019581), ('2h_WILLR', -1.2894636323011401), ('2h_ULTOSC', 1.6171715147861818), ('2h_CCI', 1.6759748000211567), ('2h_HT_PHASOR', 1.770966094776046)]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">[('2h_CDLMATHOLD', 0.0), ('2h_CDLDOJI', 0.0), ('2h_CDLLADDERBOTTOM', 0.0), ('2h_CDLDRAGONFLYDOJI', 0.0), ('2h_CDLGRAVESTONEDOJI', 0.0), ('2h_CDLTAKURI', 0.0), ('2h_CDLENGULFING', 0.0), ('2h_CDLKICKING', 0.0), ('2h_CDLKICKINGBYLENGTH', 0.0), ('2h_HT_SINE', 0.0), ('2h_HT_TRENDMODE', 0.0), ('2h_CDL3OUTSIDE', 0.0), ('2h_CDLDARKCLOUDCOVER', 0.0), ('2h_DX', 0.0), ('2h_CDLMORNINGSTAR', 0.0), ('2h_CDLINNECK', 0.0), ('2h_CDLCOUNTERATTACK', 0.0), ('2h_CDL3STARSINSOUTH', 0.0), ('2h_CDLEVENINGDOJISTAR', 0.0), ('2h_CDLUPSIDEGAP2CROWS', 0.0), ('2h_CDLHARAMI', 0.0), ('2h_CDLABANDONEDBABY', 0.0), ('12h_RSI', 0.0), ('12h_CDLHIKKAKE', 0.0), ('12h_CDLMATHOLD', 0.0), ('12h_CDLBREAKAWAY', 0.0), ('12h_CDLDOJI', 0.0), ('12h_TRIX', 0.0), ('12h_CDLLADDERBOTTOM', 0.0), ('12h_CDLRISEFALL3METHODS', 0.0), ('12h_CDLHANGINGMAN', 0.0), ('12h_AROONOSC', 0.0), ('12h_MFI', 0.0), ('12h_CDLCONCEALBABYSWALL', 0.0), ('12h_CDLHAMMER', 0.0), ('12h_CDLLONGLINE', 0.0), ('12h_CDLLONGLEGGEDDOJI', 0.0), ('12h_CDL3LINESTRIKE', 0.0), ('12h_CDLSTALLEDPATTERN', 0.0), ('12h_CDLSHORTLINE', 0.0), ('12h_HT_DCPHASE', 0.0), ('12h_CDL3BLACKCROWS', 0.0), ('12h_CDLKICKING', 0.0), ('12h_CDLKICKINGBYLENGTH', 0.0), ('12h_HT_TRENDMODE', 0.0), ('12h_CDLIDENTICAL3CROWS', 0.0), ('12h_CDLDARKCLOUDCOVER', 0.0), ('12h_ADX', 0.0), ('12h_DX', 0.0), ('12h_CDLINNECK', 0.0), ('12h_CDLONNECK', 0.0), ('12h_CDLBELTHOLD', 0.0), ('12h_CDLCOUNTERATTACK', 0.0), ('12h_CDL3STARSINSOUTH', 0.0), ('12h_CDLUPSIDEGAP2CROWS', 0.0), ('12h_CDLTHRUSTING', 0.0), ('12h_CDLABANDONEDBABY', 0.0), ('12h_CDLHIGHWAVE', 0.0), ('12h_CDLSTICKSANDWICH', 0.0), ('12h_CDLSEPARATINGLINES', 0.003756276823238492), ('12h_HT_SINE', 0.009257156593133383), </t>
+  </si>
+  <si>
+    <t>[('2h_CDLMATHOLD', 0.0), ('2h_CDLBREAKAWAY', 0.0), ('2h_CDLDOJISTAR', 0.0), ('2h_CDLSHOOTINGSTAR', 0.0), ('2h_CDLHIKKAKEMOD', 0.0), ('2h_CDLLADDERBOTTOM', 0.0), ('2h_CDLRISEFALL3METHODS', 0.0), ('2h_CDLGRAVESTONEDOJI', 0.0), ('2h_CDLHANGINGMAN', 0.0), ('2h_CDLTASUKIGAP', 0.0), ('2h_CDLCONCEALBABYSWALL', 0.0), ('2h_CDLXSIDEGAP3METHODS', 0.0), ('2h_CDLINVERTEDHAMMER', 0.0), ('2h_CDLADVANCEBLOCK', 0.0), ('2h_CDL2CROWS', 0.0), ('2h_CDL3LINESTRIKE', 0.0), ('2h_CDLSTALLEDPATTERN', 0.0), ('2h_CDL3BLACKCROWS', 0.0), ('2h_CDLUNIQUE3RIVER', 0.0), ('2h_CDL3WHITESOLDIERS', 0.0), ('2h_CDLKICKING', 0.0), ('2h_CDLKICKINGBYLENGTH', 0.0), ('2h_CDLIDENTICAL3CROWS', 0.0), ('2h_CDLTRISTAR', 0.0), ('2h_CDL3OUTSIDE', 0.0), ('2h_CDLMATCHINGLOW', 0.0), ('2h_CDLGAPSIDESIDEWHITE', 0.0), ('2h_CDLDARKCLOUDCOVER', 0.0), ('2h_CDLMORNINGSTAR', 0.0), ('2h_CDL3INSIDE', 0.0), ('2h_CDLINNECK', 0.0), ('2h_CDLONNECK', 0.0), ('2h_CDLCOUNTERATTACK', 0.0), ('2h_CDLHARAMICROSS', 0.0), ('2h_CDL3STARSINSOUTH', 0.0), ('2h_CDLEVENINGDOJISTAR', 0.0), ('2h_CDLMORNINGDOJISTAR', 0.0), ('2h_CDLUPSIDEGAP2CROWS', 0.0), ('2h_CDLSEPARATINGLINES', 0.0), ('2h_CDLTHRUSTING', 0.0), ('2h_CDLHOMINGPIGEON', 0.0), ('2h_CDLPIERCING', 0.0), ('2h_CDLABANDONEDBABY', 0.0), ('2h_CDLEVENINGSTAR', 0.0), ('2h_CDLSTICKSANDWICH', 0.0), ('12h_CDLMATHOLD', 0.0), ('12h_CDLBREAKAWAY', 0.0), ('12h_CDLDOJISTAR', 0.0), ('12h_CDLSHOOTINGSTAR', 0.0), ('12h_CDLHIKKAKEMOD', 0.0), ('12h_CDLLADDERBOTTOM', 0.0), ('12h_CDLRISEFALL3METHODS', 0.0), ('12h_CDLGRAVESTONEDOJI', 0.0), ('12h_CDLTASUKIGAP', 0.0), ('12h_CDLCONCEALBABYSWALL', 0.0), ('12h_CDLXSIDEGAP3METHODS', 0.0), ('12h_CDLHAMMER', 0.0), ('12h_CDLINVERTEDHAMMER', 0.0), ('12h_CDLADVANCEBLOCK', 0.0), ('12h_CDL2CROWS', 0.0), ('12h_CDL3LINESTRIKE', 0.0), ('12h_CDLSTALLEDPATTERN', 0.0), ('12h_CDLTAKURI', 0.0), ('12h_CDL3BLACKCROWS', 0.0), ('12h_CDLUNIQUE3RIVER', 0.0), ('12h_CDL3WHITESOLDIERS', 0.0), ('12h_CDLENGULFING', 0.0), ('12h_CDLKICKING', 0.0), ('12h_CDLKICKINGBYLENGTH', 0.0), ('12h_CDLIDENTICAL3CROWS', 0.0), ('12h_CDLTRISTAR', 0.0), ('12h_CDL3OUTSIDE', 0.0), ('12h_CDLMATCHINGLOW', 0.0), ('12h_CDLGAPSIDESIDEWHITE', 0.0), ('12h_CDLDARKCLOUDCOVER', 0.0), ('12h_CDLMORNINGSTAR', 0.0), ('12h_CDL3INSIDE', 0.0), ('12h_CDLINNECK', 0.0), ('12h_CDLONNECK', 0.0), ('12h_CDLCOUNTERATTACK', 0.0), ('12h_CDLHARAMICROSS', 0.0), ('12h_CDL3STARSINSOUTH', 0.0), ('12h_CDLEVENINGDOJISTAR', 0.0), ('12h_CDLMORNINGDOJISTAR', 0.0), ('12h_CDLUPSIDEGAP2CROWS', 0.0), ('12h_CDLSEPARATINGLINES', 0.0), ('12h_CDLTHRUSTING', 0.0), ('12h_CDLHOMINGPIGEON', 0.0), ('12h_CDLPIERCING', 0.0), ('12h_CDLABANDONEDBABY', 0.0), ('12h_CDLEVENINGSTAR', 0.0), ('12h_CDLSTICKSANDWICH', 0.0),</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ('12h_CDLDRAGONFLYDOJI', 3.518012812909512e-05), ('2h_CDLTAKURI', 9.580125412890372e-05), ('12h_CDLHANGINGMAN', 0.0001468801726882232), ('2h_CDLDRAGONFLYDOJI', 0.0001617033625283365), ('12h_CDLHARAMI', 0.0002115003809572444), ('12h_CDLHIGHWAVE', 0.0002187553999055074), ('12h_CDLMARUBOZU', 0.00022827024639948017), ('2h_CDLHAMMER', 0.00030258129939067215), ('12h_CDLCLOSINGMARUBOZU', 0.0004288232255992445), ('2h_CDLRICKSHAWMAN', 0.0004620246446382284), ('2h_CDLHARAMI', 0.00051373757922485), ('12h_CDLSPINNINGTOP', 0.0005219023923823332), ('2h_CDLHIGHWAVE', 0.000637526737622254), ('2h_CDLLONGLEGGEDDOJI', 0.0006498048298774242), ('12h_CDLLONGLEGGEDDOJI', 0.0006611568239867864), ('12h_HT_TRENDMODE', 0.0007084979512787184), ('12h_CDLLONGLINE', 0.0007146772518008718), ('12h_CDLRICKSHAWMAN', 0.0007711206418534955), ('2h_CDLENGULFING', 0.0009959193135586901), ('2h_CDLSPINNINGTOP', 0.0011119129509835075), ('2h_CDLDOJI', 0.0011961986306134118), ('12h_CDLHIKKAKE', 0.0012657499223417226), ('12h_CDLDOJI', 0.0013392149664783418), ('12h_CDLBELTHOLD', 0.0015052635206983822), ('12h_CDLSHORTLINE', 0.0016481563839429744), ('2h_CDLSHORTLINE', 0.0016905746869643754), ('2h_CDLHIKKAKE', 0.0019423355089722087), ('2h_CDLMARUBOZU', 0.0031294335821718472), ('2h_HT_TRENDMODE', 0.004660846299509167), ('2h_CDLLONGLINE', 0.007061793382313584), ('2h_CDLCLOSINGMARUBOZU', 0.009467846263767968), ('12h_AROONOSC', 0.011274616922037836), ('12h_HT_PHASOR', 0.01453925757417426), ('2h_CDLBELTHOLD', 0.015860810115229208), ('12h_ADX', 0.016203383738903013), ('12h_STOCHF', 0.016511767099188196), ('2h_AROONOSC', 0.016908061291068015), ('2h_DX', 0.01803200656689309), ('12h_STOCHRSI', 0.019238077601045317), ('2h_ADX', 0.020111976979412267), ('12h_STOCH', 0.020140574965023195), ('12h_DX', 0.020175840105282453), ('2h_PPO1', 0.02066708156467577), ('12h_WILLR', 0.020795609081532315), ('12h_HT_DCPERIOD', 0.02193830424419609), ('12h_HT_SINE', 0.02299586760874611), ('12h_PPO1', 0.023709791852057842), ('12h_MFI', 0.023805928918557717), ('12h_HT_DCPHASE', 0.024139527918426246), ('12h_ULTOSC', 0.0248407221451051), ('12h_CCI', 0.02489376293042076), ('2h_CCI', 0.025169240791544784), ('2h_TRIX', 0.025615212799137203), ('2h_MFI', 0.0257899889946091), ('2h_ULTOSC', 0.026231345690333495), ('2h_RSI', 0.026435036813157266), ('2h_HT_DCPERIOD', 0.026704565860606103), ('2h_HT_DCPHASE', 0.027146120558799076), ('2h_CMO', 0.027416145359273343), ('2h_PPO2', 0.027419992819313874), ('12h_CMO', 0.028032508293940425), ('12h_PPO2', 0.02822661828188017), ('2h_STOCHRSI', 0.02833109695704975), ('2h_HT_SINE', 0.028432282881418906), ('12h_RSI', 0.029731494849986814), ('2h_HT_PHASOR', 0.03084594654547924), ('12h_TRIX', 0.03149020505978931), ('2h_STOCH', 0.03200496016540793), ('2h_WILLR', 0.03902513621516563), ('2h_STOCHF', 0.044683942106425005)]</t>
+  </si>
+  <si>
+    <t>[('2h_CDLMATHOLD', 0.0), ('2h_CDLKICKING', 0.0), ('2h_CDLKICKINGBYLENGTH', 0.0), ('2h_CDLCOUNTERATTACK', 0.0), ('2h_CDL3STARSINSOUTH', 0.0), ('2h_CDLUPSIDEGAP2CROWS', 0.0), ('2h_CDLABANDONEDBABY', 0.0), ('12h_CDLMATHOLD', 0.0), ('12h_CDLBREAKAWAY', 0.0), ('12h_CDLLADDERBOTTOM', 0.0), ('12h_CDLCONCEALBABYSWALL', 0.0), ('12h_CDL3BLACKCROWS', 0.0), ('12h_CDLKICKING', 0.0), ('12h_CDLKICKINGBYLENGTH', 0.0), ('12h_CDLIDENTICAL3CROWS', 0.0), ('12h_CDLINNECK', 0.0), ('12h_CDLONNECK', 0.0), ('12h_CDLCOUNTERATTACK', 0.0), ('12h_CDL3STARSINSOUTH', 0.0), ('12h_CDLUPSIDEGAP2CROWS', 0.0), ('12h_CDLABANDONEDBABY', 0.0), ('12h_CDLDOJISTAR', 0.0007051941056163136), ('2h_HT_TRENDMODE', -0.00129857795600552), ('2h_CDLEVENINGSTAR', 0.0013371376004388535), ('2h_CDLGRAVESTONEDOJI', 0.0019070132642409199), ('12h_AROONOSC', -0.0020821099430312928), ('12h_MFI', -0.002446253257620162), ('12h_CDLXSIDEGAP3METHODS', 0.002902839595455786), ('2h_HT_SINE', -0.002979713423727426), ('12h_HT_SINE', 0.00324508094207634), ('2h_CDL3OUTSIDE', 0.005104129885975972), ('12h_CDLSTALLEDPATTERN', -0.005504238746958379), ('12h_HT_TRENDMODE', 0.0057217675997346396), ('12h_RSI', 0.007111135210351718),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[('2h_CDLMATHOLD', 0.0), ('2h_CDLBREAKAWAY', 0.0), ('2h_CDLDOJISTAR', 0.0), ('2h_CDLHIKKAKEMOD', 0.0), ('2h_CDLLADDERBOTTOM', 0.0), ('2h_CDLRISEFALL3METHODS', 0.0), ('2h_CDLCONCEALBABYSWALL', 0.0), ('2h_CDL2CROWS', 0.0), ('2h_CDL3LINESTRIKE', 0.0), ('2h_CDL3BLACKCROWS', 0.0), ('2h_CDLUNIQUE3RIVER', 0.0), ('2h_CDLKICKING', 0.0), ('2h_CDLKICKINGBYLENGTH', 0.0), ('2h_CDLIDENTICAL3CROWS', 0.0), ('2h_CDLTRISTAR', 0.0), ('2h_CDLGAPSIDESIDEWHITE', 0.0), ('2h_CDLDARKCLOUDCOVER', 0.0), ('2h_CDLMORNINGSTAR', 0.0), ('2h_CDLINNECK', 0.0), ('2h_CDLONNECK', 0.0), ('2h_CDLCOUNTERATTACK', 0.0), ('2h_CDL3STARSINSOUTH', 0.0), ('2h_CDLEVENINGDOJISTAR', 0.0), ('2h_CDLMORNINGDOJISTAR', 0.0), ('2h_CDLUPSIDEGAP2CROWS', 0.0), ('2h_CDLHOMINGPIGEON', 0.0), ('2h_CDLPIERCING', 0.0), ('2h_CDLABANDONEDBABY', 0.0), ('2h_CDLSTICKSANDWICH', 0.0), ('12h_CDLMATHOLD', 0.0), ('12h_CDLBREAKAWAY', 0.0), ('12h_CDLHIKKAKEMOD', 0.0), ('12h_CDLLADDERBOTTOM', 0.0), ('12h_CDLRISEFALL3METHODS', 0.0), ('12h_CDLTASUKIGAP', 0.0), ('12h_CDLCONCEALBABYSWALL', 0.0), ('12h_CDLINVERTEDHAMMER', 0.0), ('12h_CDL2CROWS', 0.0), ('12h_CDL3LINESTRIKE', 0.0), ('12h_CDLSTALLEDPATTERN', 0.0), ('12h_CDL3BLACKCROWS', 0.0), ('12h_CDLUNIQUE3RIVER', 0.0), ('12h_CDL3WHITESOLDIERS', 0.0), ('12h_CDLKICKING', 0.0), ('12h_CDLKICKINGBYLENGTH', 0.0), ('12h_CDLIDENTICAL3CROWS', 0.0), ('12h_CDLTRISTAR', 0.0), ('12h_CDLGAPSIDESIDEWHITE', 0.0), ('12h_CDLMORNINGSTAR', 0.0), ('12h_CDLINNECK', 0.0), ('12h_CDLONNECK', 0.0), ('12h_CDLCOUNTERATTACK', 0.0), ('12h_CDL3STARSINSOUTH', 0.0), ('12h_CDLEVENINGDOJISTAR', 0.0), ('12h_CDLMORNINGDOJISTAR', 0.0), ('12h_CDLUPSIDEGAP2CROWS', 0.0), ('12h_CDLTHRUSTING', 0.0), ('12h_CDLHOMINGPIGEON', 0.0), ('12h_CDLPIERCING', 0.0), ('12h_CDLABANDONEDBABY', 0.0), ('12h_CDLEVENINGSTAR', 0.0), ('12h_CDLSTICKSANDWICH', 0.0), ('2h_CDLHARAMICROSS', 0.0017391085), ('2h_CDLXSIDEGAP3METHODS', 0.0026703614), ('2h_CDL3WHITESOLDIERS', 0.0049547385), </t>
   </si>
 </sst>
 </file>
@@ -267,7 +351,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="36">
+  <fonts count="44">
     <font>
       <sz val="11.0"/>
       <name val="맑은 고딕"/>
@@ -456,6 +540,46 @@
       <sz val="11.0"/>
       <name val="맑은 고딕"/>
       <color rgb="FF009297"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <name val="monospace"/>
+      <color rgb="FF212121"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color theme="1"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <name val="monospace"/>
+      <color theme="1"/>
+    </font>
+    <font>
+      <sz val="9.0"/>
+      <name val="맑은 고딕"/>
+      <color theme="1"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="monospace"/>
+      <color theme="1"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="DengXian"/>
+      <color theme="1"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="MS Gothic"/>
+      <color theme="1"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Microsoft YaHei"/>
+      <color theme="1"/>
     </font>
   </fonts>
   <fills count="36">
@@ -841,7 +965,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -937,6 +1061,36 @@
     </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1258,7 +1412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -1624,14 +1778,88 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.500000"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="14.62500000" defaultRowHeight="16.500000"/>
+  <cols>
+    <col min="1" max="1" width="22.25499916" customWidth="1" outlineLevel="0"/>
+    <col min="2" max="4" width="6.00500011" customWidth="1" outlineLevel="0"/>
+    <col min="5" max="5" style="41" width="150.63000488" customWidth="1" outlineLevel="0"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="181.500000">
+      <c r="A1" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="0">
+        <v>15.3</v>
+      </c>
+      <c r="C1" s="0">
+        <v>0.589</v>
+      </c>
+      <c r="D1" s="0">
+        <v>0.517</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="297.000000">
+      <c r="A2" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="0">
+        <v>8.9</v>
+      </c>
+      <c r="C2" s="0">
+        <v>0.764</v>
+      </c>
+      <c r="D2" s="0">
+        <v>0.271</v>
+      </c>
+      <c r="E2" s="41" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="132.000000">
+      <c r="A3" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="0">
+        <v>7.89</v>
+      </c>
+      <c r="C3" s="0">
+        <v>0.726</v>
+      </c>
+      <c r="D3" s="0">
+        <v>0.358</v>
+      </c>
+      <c r="E3" s="41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="231.000000">
+      <c r="A4" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="0">
+        <v>12.57</v>
+      </c>
+      <c r="C4" s="0">
+        <v>0.618</v>
+      </c>
+      <c r="D4" s="0">
+        <v>0.469</v>
+      </c>
+      <c r="E4" s="41" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
update useful and useless feature names
</commit_message>
<xml_diff>
--- a/data/features.xlsx
+++ b/data/features.xlsx
@@ -1,32 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26311"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qin/coinx/stock/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="460" windowWidth="25760" windowHeight="11600" tabRatio="550" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
     <sheet name="Useless" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="193">
   <si>
     <t>HT_DCPERIOD</t>
   </si>
@@ -410,112 +401,442 @@
   </si>
   <si>
     <t>12h_CDLTHRUSTING</t>
+  </si>
+  <si>
+    <t>Top Useless 2h</t>
+  </si>
+  <si>
+    <t>Top Useless 12h</t>
+  </si>
+  <si>
+    <t>Top Useful 2h</t>
+  </si>
+  <si>
+    <t>Top Useful 12h</t>
+  </si>
+  <si>
+    <t>2h_HT_PHASOR</t>
+  </si>
+  <si>
+    <t>2h_STOCHF</t>
+  </si>
+  <si>
+    <t>2h_WILLR</t>
+  </si>
+  <si>
+    <t>2h_RSI</t>
+  </si>
+  <si>
+    <t>2h_CCI</t>
+  </si>
+  <si>
+    <t>2h_ULTOSC</t>
+  </si>
+  <si>
+    <t>12h_PPO1</t>
+  </si>
+  <si>
+    <t>2h_PPO2</t>
+  </si>
+  <si>
+    <t>12h_CMO</t>
+  </si>
+  <si>
+    <t>12h_CCI</t>
+  </si>
+  <si>
+    <t>2h_CMO</t>
+  </si>
+  <si>
+    <t>2h_STOCHRSI</t>
+  </si>
+  <si>
+    <t>2h_PPO1</t>
+  </si>
+  <si>
+    <t>12h_TRIX</t>
+  </si>
+  <si>
+    <t>2h_TRIX</t>
+  </si>
+  <si>
+    <t>2h_STOCH</t>
+  </si>
+  <si>
+    <t>12h_PPO2</t>
+  </si>
+  <si>
+    <t>2h_HT_DCPHASE</t>
+  </si>
+  <si>
+    <t>2h_HT_DCPERIOD</t>
+  </si>
+  <si>
+    <t>2h_CDLBELTHOLD</t>
+  </si>
+  <si>
+    <t>12h_RSI</t>
+  </si>
+  <si>
+    <t>2h_MFI</t>
+  </si>
+  <si>
+    <t>12h_ULTOSC</t>
+  </si>
+  <si>
+    <t>2h_HT_SINE</t>
+  </si>
+  <si>
+    <t>12h_HT_DCPERIOD</t>
+  </si>
+  <si>
+    <t>12h_MFI</t>
+  </si>
+  <si>
+    <t>2h_ADX</t>
+  </si>
+  <si>
+    <t>12h_STOCH</t>
+  </si>
+  <si>
+    <t>12h_HT_DCPHASE</t>
+  </si>
+  <si>
+    <t>12h_HT_SINE</t>
+  </si>
+  <si>
+    <t>12h_WILLR</t>
+  </si>
+  <si>
+    <t>2h_CDLEVENINGSTAR</t>
+  </si>
+  <si>
+    <t>12h_STOCHRSI</t>
+  </si>
+  <si>
+    <t>2h_AROONOSC</t>
+  </si>
+  <si>
+    <t>New FEa</t>
+  </si>
+  <si>
+    <t>New Features</t>
+  </si>
+  <si>
+    <t>inphase, quadrature = HT_PHASOR(close)</t>
+  </si>
+  <si>
+    <t>fastk, fastd = STOCHF</t>
+  </si>
+  <si>
+    <t>inphase, quadrature = HT_PHASOR</t>
+  </si>
+  <si>
+    <t>WILLR double period</t>
+  </si>
+  <si>
+    <t>RSI doule period</t>
+  </si>
+  <si>
+    <t>CCI doule period</t>
+  </si>
+  <si>
+    <t>ULTOSC double period</t>
+  </si>
+  <si>
+    <t>CMO double period</t>
+  </si>
+  <si>
+    <t>STOCHRSI doule period</t>
+  </si>
+  <si>
+    <t>TRIX double period</t>
+  </si>
+  <si>
+    <t>STOCHRSI double period</t>
+  </si>
+  <si>
+    <t>slowk, slowd = STOCH</t>
+  </si>
+  <si>
+    <t>MFI doub;e [erop</t>
+  </si>
+  <si>
+    <t>MFI double period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PPO 1 </t>
+  </si>
+  <si>
+    <t>PPO 4</t>
+  </si>
+  <si>
+    <t>sine, leadsine = HT_SINE</t>
+  </si>
+  <si>
+    <t>ADX double</t>
+  </si>
+  <si>
+    <t>AROONOSC doule</t>
+  </si>
+  <si>
+    <t>AROONOSC double</t>
+  </si>
+  <si>
+    <t>DX double</t>
+  </si>
+  <si>
+    <t>fastk, fastd = STOCHF double</t>
+  </si>
+  <si>
+    <t>slowk, slowd = STOCH double</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF009900"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>ULTOSC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t xml:space="preserve"> double period</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF009900"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>ULTOSC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF009900"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t xml:space="preserve"> double period</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="64" formatCode="&quot;$&quot;#,##0;\\\-&quot;$&quot;#,##0"/>
+  </numFmts>
+  <fonts count="36">
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
-    </font>
-    <font>
-      <sz val="8"/>
+    </font>
+    <font>
+      <sz val="8.0"/>
+      <name val="맑은 고딕"/>
       <color rgb="FF000000"/>
-      <name val="맑은 고딕"/>
-    </font>
-    <font>
-      <sz val="11"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
       <color rgb="FFFF0000"/>
-      <name val="맑은 고딕"/>
-    </font>
-    <font>
-      <sz val="11"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
       <color rgb="FF7DCD00"/>
-      <name val="맑은 고딕"/>
-    </font>
-    <font>
-      <sz val="11"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
       <color rgb="FFFC6600"/>
-      <name val="맑은 고딕"/>
-    </font>
-    <font>
-      <sz val="11"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
       <color rgb="FFFFFF00"/>
-      <name val="맑은 고딕"/>
-    </font>
-    <font>
-      <sz val="11"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
       <color rgb="FFFF0066"/>
-      <name val="맑은 고딕"/>
-    </font>
-    <font>
-      <sz val="11"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
       <color rgb="FF770055"/>
-      <name val="맑은 고딕"/>
-    </font>
-    <font>
-      <sz val="11"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
       <color rgb="FF008080"/>
-      <name val="맑은 고딕"/>
-    </font>
-    <font>
-      <sz val="11"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
       <color rgb="FF009900"/>
-      <name val="맑은 고딕"/>
-    </font>
-    <font>
-      <sz val="11"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
       <color rgb="FF36B700"/>
-      <name val="맑은 고딕"/>
-    </font>
-    <font>
-      <sz val="11"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
       <color rgb="FFFCCC00"/>
-      <name val="맑은 고딕"/>
-    </font>
-    <font>
-      <sz val="11"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
       <color rgb="FF4D009A"/>
-      <name val="맑은 고딕"/>
-    </font>
-    <font>
-      <sz val="11"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
       <color rgb="FF00007E"/>
-      <name val="맑은 고딕"/>
-    </font>
-    <font>
-      <sz val="11"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
       <color rgb="FF003A9A"/>
-      <name val="맑은 고딕"/>
-    </font>
-    <font>
-      <sz val="11"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
       <color rgb="FF009297"/>
-      <name val="맑은 고딕"/>
-    </font>
-    <font>
-      <sz val="11"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Microsoft YaHei"/>
       <color theme="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color theme="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color theme="10"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color theme="11"/>
+    </font>
+    <font>
+      <sz val="18.0"/>
+      <name val="맑은 고딕"/>
+      <color theme="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15.0"/>
+      <name val="맑은 고딕"/>
+      <color theme="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.0"/>
+      <name val="맑은 고딕"/>
+      <color theme="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color theme="3"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FF3F3F76"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FF3F3F3F"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FFFA7D00"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FFFFFFFF"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FFFA7D00"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FF006100"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FF9C0006"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FF9C6500"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color theme="0"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color theme="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FF7F7F7F"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
       <name val="Microsoft YaHei"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
-      <charset val="129"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -523,8 +844,194 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599990"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599990"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599990"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599990"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599990"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599990"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -547,85 +1054,389 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFACCCEA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.399980"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="64" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="6" applyAlignment="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="7" applyAlignment="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="6" applyAlignment="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="8" applyAlignment="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="10" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="11" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="12" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="13" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="14" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="15" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="16" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="17" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="18" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="19" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="20" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="21" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="22" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="25" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="26" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="28" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="29" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="30" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="31" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="32" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="33" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="20% - Accent2" xfId="29" builtinId="34"/>
+    <cellStyle name="20% - Accent3" xfId="33" builtinId="38"/>
+    <cellStyle name="20% - Accent4" xfId="37" builtinId="42"/>
+    <cellStyle name="20% - Accent5" xfId="41" builtinId="46"/>
+    <cellStyle name="20% - Accent6" xfId="45" builtinId="50"/>
+    <cellStyle name="40% - Accent1" xfId="26" builtinId="31"/>
+    <cellStyle name="40% - Accent2" xfId="30" builtinId="35"/>
+    <cellStyle name="40% - Accent3" xfId="34" builtinId="39"/>
+    <cellStyle name="40% - Accent4" xfId="38" builtinId="43"/>
+    <cellStyle name="40% - Accent5" xfId="42" builtinId="47"/>
+    <cellStyle name="40% - Accent6" xfId="46" builtinId="51"/>
+    <cellStyle name="60% - Accent1" xfId="27" builtinId="32"/>
+    <cellStyle name="60% - Accent2" xfId="31" builtinId="36"/>
+    <cellStyle name="60% - Accent3" xfId="35" builtinId="40"/>
+    <cellStyle name="60% - Accent4" xfId="39" builtinId="44"/>
+    <cellStyle name="60% - Accent5" xfId="43" builtinId="48"/>
+    <cellStyle name="60% - Accent6" xfId="47" builtinId="52"/>
+    <cellStyle name="Accent1" xfId="24" builtinId="29"/>
+    <cellStyle name="Accent2" xfId="28" builtinId="33"/>
+    <cellStyle name="Accent3" xfId="32" builtinId="37"/>
+    <cellStyle name="Accent4" xfId="36" builtinId="41"/>
+    <cellStyle name="Accent5" xfId="40" builtinId="45"/>
+    <cellStyle name="Accent6" xfId="44" builtinId="49"/>
+    <cellStyle name="Bad" xfId="22" builtinId="27"/>
+    <cellStyle name="Calculation" xfId="17" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="18" builtinId="23"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Comment" xfId="8" builtinId="10"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Currency[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Explanatory Text" xfId="48" builtinId="53"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="21" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Input" xfId="15" builtinId="20"/>
+    <cellStyle name="Linked Cell" xfId="19" builtinId="24"/>
+    <cellStyle name="Neutral" xfId="23" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="16" builtinId="21"/>
+    <cellStyle name="Percentage" xfId="3" builtinId="5"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="Title 1" xfId="11" builtinId="16"/>
+    <cellStyle name="Title 2" xfId="12" builtinId="17"/>
+    <cellStyle name="Title 3" xfId="13" builtinId="18"/>
+    <cellStyle name="Title 4" xfId="14" builtinId="19"/>
+    <cellStyle name="Total" xfId="20" builtinId="25"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -891,58 +1702,58 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="16.500000"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="22.83203125" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" customWidth="1"/>
-    <col min="7" max="7" width="21.83203125" customWidth="1"/>
-    <col min="8" max="8" width="22.83203125" customWidth="1"/>
-    <col min="9" max="9" width="24.83203125" customWidth="1"/>
-    <col min="10" max="10" width="24.5" customWidth="1"/>
+    <col min="1" max="1" width="2.63000011" customWidth="1" outlineLevel="0"/>
+    <col min="2" max="2" width="21.62999916" customWidth="1" outlineLevel="0"/>
+    <col min="3" max="3" width="22.87999916" customWidth="1" outlineLevel="0"/>
+    <col min="4" max="4" width="24.37999916" customWidth="1" outlineLevel="0"/>
+    <col min="5" max="5" width="21.62999916" customWidth="1" outlineLevel="0"/>
+    <col min="6" max="6" width="18.62999916" customWidth="1" outlineLevel="0"/>
+    <col min="7" max="7" width="21.87999916" customWidth="1" outlineLevel="0"/>
+    <col min="8" max="8" width="22.87999916" customWidth="1" outlineLevel="0"/>
+    <col min="9" max="9" width="24.87999916" customWidth="1" outlineLevel="0"/>
+    <col min="10" max="10" width="24.50499916" customWidth="1" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1">
+    <row r="1" spans="1:10">
+      <c r="B1" s="0">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="0">
         <v>2</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="0">
         <v>3</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="0">
         <v>4</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="0">
         <v>5</v>
       </c>
-      <c r="G1">
+      <c r="G1" s="0">
         <v>6</v>
       </c>
-      <c r="H1">
+      <c r="H1" s="0">
         <v>7</v>
       </c>
-      <c r="I1">
+      <c r="I1" s="0">
         <v>8</v>
       </c>
-      <c r="J1">
+      <c r="J1" s="0">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:10">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -973,8 +1784,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:10">
+      <c r="A3" s="0">
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -1005,8 +1816,8 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:10">
+      <c r="A4" s="0">
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -1037,7 +1848,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -1048,8 +1859,8 @@
       <c r="I5" s="17"/>
       <c r="J5" s="18"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:10">
+      <c r="A6" s="0">
         <v>4</v>
       </c>
       <c r="B6" s="9" t="s">
@@ -1080,8 +1891,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:10">
+      <c r="A7" s="0">
         <v>5</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -1112,8 +1923,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:10">
+      <c r="A8" s="0">
         <v>6</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -1144,7 +1955,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
@@ -1155,8 +1966,8 @@
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:10">
+      <c r="A10" s="0">
         <v>7</v>
       </c>
       <c r="B10" s="12" t="s">
@@ -1187,8 +1998,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:10">
+      <c r="A11" s="0">
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -1219,8 +2030,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:10">
+      <c r="A12" s="0">
         <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -1253,357 +2064,396 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.66406250" defaultRowHeight="16.500000"/>
   <cols>
-    <col min="1" max="1" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6" customWidth="1"/>
-    <col min="5" max="5" width="150.6640625" style="19" customWidth="1"/>
+    <col min="1" max="1" width="26.50499916" customWidth="1" outlineLevel="0"/>
+    <col min="2" max="2" width="27.87999916" customWidth="1" outlineLevel="0"/>
+    <col min="3" max="3" width="6.00500011" customWidth="1" outlineLevel="0"/>
+    <col min="4" max="4" width="20.87999916" customWidth="1" outlineLevel="0"/>
+    <col min="5" max="5" style="19" width="19.50499916" customWidth="1" outlineLevel="0"/>
+    <col min="6" max="6" width="38.88000107" customWidth="1" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="20" t="s">
-        <v>81</v>
+        <v>129</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="D17" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" s="0" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="24" spans="1:6">
+      <c r="A24" s="0" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="16.500000"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
pick up useless feature names
</commit_message>
<xml_diff>
--- a/data/features.xlsx
+++ b/data/features.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="540" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="211">
   <si>
     <t>HT_DCPERIOD</t>
   </si>
@@ -625,6 +625,237 @@
         <rFont val="맑은 고딕"/>
       </rPr>
       <t xml:space="preserve"> double period</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>12h_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>CDL3LINESTRIKE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>12h_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>CDL3STARSINSOUTH</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>12h_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>CDLABANDONEDBABY</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2h_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>CDLCONCEALBABYSWALL</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0066"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>12h_CDLBREAKAWAY</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>12h_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>CDLCONCEALBABYSWALL</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2h_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>CDLCONCEALBABYSWALL</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>12h_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>CDLCOUNTERATTACK</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>12h_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>CDLINNECK</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>12h_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>CDLKICKING</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>12h_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>CDLKICKINGBYLENGTH</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>12h_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>CDLLADDERBOTTOM</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>12h_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>CDLMATHOLD</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>12h_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>CDLMORNINGSTAR</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>12h_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>CDLONNECK</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>12h_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>CDLSTICKSANDWICH</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>12h_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>CDLTRISTAR</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>12h_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>CDLUPSIDEGAP2CROWS</t>
     </r>
   </si>
 </sst>
@@ -811,20 +1042,20 @@
       <color theme="0"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <name val="맑은 고딕"/>
+      <i/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FF7F7F7F"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="Microsoft YaHei"/>
       <color theme="1"/>
     </font>
     <font>
-      <i/>
-      <sz val="11.0"/>
-      <name val="맑은 고딕"/>
-      <color rgb="FF7F7F7F"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11.0"/>
-      <name val="Microsoft YaHei"/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
       <color theme="1"/>
     </font>
   </fonts>
@@ -1236,10 +1467,10 @@
     <xf numFmtId="0" fontId="32" fillId="10" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="11" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="12" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="13" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
@@ -1248,10 +1479,10 @@
     <xf numFmtId="0" fontId="32" fillId="14" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="15" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="16" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="17" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
@@ -1260,10 +1491,10 @@
     <xf numFmtId="0" fontId="32" fillId="18" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="19" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="20" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="21" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
@@ -1272,10 +1503,10 @@
     <xf numFmtId="0" fontId="32" fillId="22" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="25" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
@@ -1284,10 +1515,10 @@
     <xf numFmtId="0" fontId="32" fillId="26" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="27" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="28" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="29" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
@@ -1296,20 +1527,20 @@
     <xf numFmtId="0" fontId="32" fillId="30" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="31" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="32" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="33" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1373,16 +1604,19 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2073,8 +2307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView topLeftCell="A13" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.66406250" defaultRowHeight="16.500000"/>
@@ -2094,21 +2328,21 @@
       <c r="B1" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="24" t="s">
         <v>120</v>
       </c>
       <c r="D2" s="0" t="s">
@@ -2117,13 +2351,13 @@
       <c r="E2" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="22" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="0" t="s">
-        <v>110</v>
+      <c r="A3" s="23" t="s">
+        <v>193</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>126</v>
@@ -2134,13 +2368,13 @@
       <c r="E3" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="22" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="0" t="s">
-        <v>101</v>
+      <c r="A4" s="23" t="s">
+        <v>194</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>87</v>
@@ -2151,12 +2385,12 @@
       <c r="E4" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="22" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="24" t="s">
         <v>125</v>
       </c>
       <c r="B5" s="0" t="s">
@@ -2168,16 +2402,16 @@
       <c r="E5" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="22" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>117</v>
+      <c r="A6" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>199</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>136</v>
@@ -2185,13 +2419,13 @@
       <c r="E6" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="22" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="0" t="s">
-        <v>91</v>
+      <c r="A7" s="24" t="s">
+        <v>197</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>86</v>
@@ -2202,15 +2436,15 @@
       <c r="E7" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="22" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="B8" s="0" t="s">
+      <c r="A8" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="B8" s="24" t="s">
         <v>105</v>
       </c>
       <c r="D8" s="0" t="s">
@@ -2219,15 +2453,15 @@
       <c r="E8" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="22" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="B9" s="0" t="s">
+      <c r="A9" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="B9" s="24" t="s">
         <v>123</v>
       </c>
       <c r="D9" s="0" t="s">
@@ -2236,15 +2470,15 @@
       <c r="E9" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="22" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="24" t="s">
         <v>108</v>
       </c>
       <c r="D10" s="0" t="s">
@@ -2253,15 +2487,15 @@
       <c r="E10" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F10" s="22" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="24" t="s">
         <v>113</v>
       </c>
       <c r="D11" s="0" t="s">
@@ -2270,15 +2504,15 @@
       <c r="E11" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="22" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="B12" s="0" t="s">
+      <c r="A12" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="B12" s="24" t="s">
         <v>115</v>
       </c>
       <c r="D12" s="0" t="s">
@@ -2287,13 +2521,13 @@
       <c r="E12" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="F12" s="22" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="0" t="s">
-        <v>95</v>
+      <c r="A13" s="23" t="s">
+        <v>202</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>107</v>
@@ -2304,13 +2538,13 @@
       <c r="E13" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="22" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="0" t="s">
-        <v>96</v>
+      <c r="A14" s="23" t="s">
+        <v>203</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>84</v>
@@ -2321,13 +2555,13 @@
       <c r="E14" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="22" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="0" t="s">
-        <v>92</v>
+      <c r="A15" s="23" t="s">
+        <v>204</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>85</v>
@@ -2338,13 +2572,13 @@
       <c r="E15" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="F15" s="23" t="s">
+      <c r="F15" s="22" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="0" t="s">
-        <v>90</v>
+      <c r="A16" s="23" t="s">
+        <v>205</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>104</v>
@@ -2352,13 +2586,13 @@
       <c r="D16" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="F16" s="23" t="s">
+      <c r="F16" s="22" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="0" t="s">
-        <v>124</v>
+      <c r="A17" s="23" t="s">
+        <v>206</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>83</v>
@@ -2366,13 +2600,13 @@
       <c r="D17" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="F17" s="23" t="s">
+      <c r="F17" s="22" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="0" t="s">
-        <v>99</v>
+      <c r="A18" s="23" t="s">
+        <v>207</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>106</v>
@@ -2382,7 +2616,7 @@
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="24" t="s">
         <v>109</v>
       </c>
       <c r="B19" s="0" t="s">
@@ -2393,7 +2627,7 @@
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="24" t="s">
         <v>111</v>
       </c>
       <c r="B20" s="0" t="s">
@@ -2404,8 +2638,8 @@
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="0" t="s">
-        <v>112</v>
+      <c r="A21" s="23" t="s">
+        <v>208</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>116</v>
@@ -2415,24 +2649,24 @@
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="24" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="0" t="s">
-        <v>118</v>
+      <c r="A23" s="23" t="s">
+        <v>209</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="0" t="s">
-        <v>102</v>
+      <c r="A24" s="23" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>